<commit_message>
improve naming and results presentation
</commit_message>
<xml_diff>
--- a/ConsSustainingAnalysis/results/overview semi-automated analysis.xlsx
+++ b/ConsSustainingAnalysis/results/overview semi-automated analysis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\figures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\git\conssus\ConsSustainingAnalysis\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="25">
   <si>
     <t>addToClass_encapsulates_Feature</t>
   </si>
@@ -77,18 +77,12 @@
     <t>Impro</t>
   </si>
   <si>
-    <t>? (braun+gr)</t>
-  </si>
-  <si>
     <t>Sust</t>
   </si>
   <si>
     <t>strongly improving</t>
   </si>
   <si>
-    <t>should be + (there is a bug in AGG explaining why a dependency is reported)</t>
-  </si>
-  <si>
     <t>dependencies are real (and point to a case of sus. but not directly sus.)</t>
   </si>
   <si>
@@ -101,7 +95,10 @@
     <t>not improving but we cannot show it</t>
   </si>
   <si>
-    <t>could potentially be fixed with a new result</t>
+    <t>should be + (there is a bug in AGG leading to this -)</t>
+  </si>
+  <si>
+    <t>not improving but we cannot show it - but could potentially be changed with a new result</t>
   </si>
 </sst>
 </file>
@@ -118,7 +115,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,12 +131,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -192,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -202,7 +193,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,23 +478,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:V15"/>
+  <dimension ref="D1:V14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.26953125" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="2" max="2" width="1.54296875" customWidth="1"/>
+    <col min="3" max="3" width="2" customWidth="1"/>
+    <col min="4" max="4" width="29.90625" customWidth="1"/>
     <col min="15" max="15" width="4.1796875" customWidth="1"/>
     <col min="19" max="19" width="4.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="4:22" x14ac:dyDescent="0.35">
       <c r="E1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J1" t="s">
         <v>16</v>
@@ -516,7 +508,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="4:22" x14ac:dyDescent="0.35">
       <c r="E2" t="s">
         <v>9</v>
       </c>
@@ -566,8 +558,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
+    <row r="3" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -585,7 +577,7 @@
       <c r="I3" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="K3" t="s">
@@ -615,18 +607,18 @@
       <c r="U3" t="s">
         <v>3</v>
       </c>
-      <c r="V3" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+      <c r="V3" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G4" t="s">
@@ -647,7 +639,7 @@
       <c r="L4" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="N4" t="s">
@@ -656,7 +648,7 @@
       <c r="P4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="R4" t="s">
@@ -665,30 +657,30 @@
       <c r="T4" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="V4" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
+      <c r="U4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G5" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="4" t="s">
+      <c r="H5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="J5" t="s">
@@ -700,33 +692,33 @@
       <c r="L5" t="s">
         <v>1</v>
       </c>
-      <c r="M5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="N5" s="5" t="s">
+      <c r="M5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="P5" t="s">
         <v>3</v>
       </c>
-      <c r="Q5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="T5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="U5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="V5" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
+      <c r="Q5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="T5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
         <v>5</v>
       </c>
       <c r="E6" t="s">
@@ -738,7 +730,7 @@
       <c r="G6" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="I6" t="s">
@@ -747,7 +739,7 @@
       <c r="J6" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="L6" t="s">
@@ -762,7 +754,7 @@
       <c r="P6" t="s">
         <v>2</v>
       </c>
-      <c r="Q6" s="4" t="s">
+      <c r="Q6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="R6" t="s">
@@ -771,15 +763,15 @@
       <c r="T6" t="s">
         <v>3</v>
       </c>
-      <c r="U6" s="5" t="s">
+      <c r="U6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="V6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
+    <row r="7" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
         <v>6</v>
       </c>
       <c r="E7" t="s">
@@ -791,7 +783,7 @@
       <c r="G7" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="I7" t="s">
@@ -815,7 +807,7 @@
       <c r="P7" t="s">
         <v>2</v>
       </c>
-      <c r="Q7" s="4" t="s">
+      <c r="Q7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="R7" t="s">
@@ -831,8 +823,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
+    <row r="8" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -844,10 +836,10 @@
       <c r="G8" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" s="4" t="s">
+      <c r="H8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="J8" t="s">
@@ -862,30 +854,30 @@
       <c r="M8" t="s">
         <v>2</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="P8" t="s">
         <v>3</v>
       </c>
-      <c r="Q8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="R8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="T8" s="9" t="s">
+      <c r="Q8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="T8" s="8" t="s">
         <v>3</v>
       </c>
       <c r="U8" t="s">
         <v>3</v>
       </c>
-      <c r="V8" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
+      <c r="V8" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -897,10 +889,10 @@
       <c r="G9" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" s="4" t="s">
+      <c r="H9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="J9" t="s">
@@ -915,66 +907,64 @@
       <c r="M9" t="s">
         <v>2</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="4" t="s">
         <v>2</v>
       </c>
       <c r="P9" t="s">
         <v>3</v>
       </c>
-      <c r="Q9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="R9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="T9" s="9" t="s">
+      <c r="Q9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="T9" s="8" t="s">
         <v>3</v>
       </c>
       <c r="U9" t="s">
         <v>3</v>
       </c>
-      <c r="V9" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="V9" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="4:22" x14ac:dyDescent="0.35">
       <c r="E11" s="1"/>
       <c r="F11" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q11" s="8"/>
-      <c r="R11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+      <c r="M11" s="5"/>
+      <c r="N11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="4:22" x14ac:dyDescent="0.35">
       <c r="E12" s="2"/>
       <c r="F12" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q12" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="R12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="7"/>
+      <c r="N12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="E13" s="3"/>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="N13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="M14" s="4"/>
+      <c r="N14" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="E13" s="4"/>
-      <c r="F13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="E14" s="6"/>
-      <c r="F14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="E15" s="5"/>
-      <c r="F15" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>